<commit_message>
start script to load age composition by geo area data
</commit_message>
<xml_diff>
--- a/originals/files catalog.xlsx
+++ b/originals/files catalog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OWNER\Dropbox\projects\local_authorities_in_Israel\originals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34D47B6E-6EB0-46C1-AAE0-5C1F7B38329D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4517E3F4-D254-4BD9-B779-6370F51180F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -598,22 +598,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -900,19 +907,19 @@
   <dimension ref="A1:H131"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5:E25"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F84" sqref="F84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="57.33203125" customWidth="1"/>
-    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
+    <col min="6" max="6" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>74</v>
       </c>
@@ -938,14 +945,14 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="2"/>
       <c r="D2">
         <v>2019</v>
       </c>
@@ -953,10 +960,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
       <c r="D3">
         <v>2018</v>
       </c>
@@ -964,10 +971,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
       <c r="D4">
         <v>2017</v>
       </c>
@@ -975,1417 +982,1477 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="2"/>
       <c r="D5">
         <v>2019</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="3" t="s">
         <v>72</v>
       </c>
       <c r="F5">
         <v>2019</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="1"/>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="2"/>
       <c r="D6">
         <v>2018</v>
       </c>
-      <c r="E6" s="2"/>
+      <c r="E6" s="3"/>
       <c r="F6">
         <v>2018</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="1"/>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="2"/>
       <c r="D7">
         <v>2017</v>
       </c>
-      <c r="E7" s="2"/>
+      <c r="E7" s="3"/>
       <c r="F7">
         <v>2017</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="1"/>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="2"/>
       <c r="D8">
         <v>2016</v>
       </c>
-      <c r="E8" s="2"/>
+      <c r="E8" s="3"/>
       <c r="F8">
         <v>2016</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="1"/>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="2"/>
       <c r="D9">
         <v>2015</v>
       </c>
-      <c r="E9" s="2"/>
+      <c r="E9" s="3"/>
       <c r="F9">
         <v>2015</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="1"/>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="2"/>
       <c r="D10">
         <v>2014</v>
       </c>
-      <c r="E10" s="2"/>
+      <c r="E10" s="3"/>
       <c r="F10">
         <v>2014</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="1"/>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="2"/>
       <c r="D11">
         <v>2013</v>
       </c>
-      <c r="E11" s="2"/>
+      <c r="E11" s="3"/>
       <c r="F11">
         <v>2013</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="1"/>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="2"/>
       <c r="D12">
         <v>2012</v>
       </c>
-      <c r="E12" s="2"/>
+      <c r="E12" s="3"/>
       <c r="F12">
         <v>2012</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="1"/>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="2"/>
       <c r="D13">
         <v>2011</v>
       </c>
-      <c r="E13" s="2"/>
+      <c r="E13" s="3"/>
       <c r="F13">
         <v>2011</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="1"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="2"/>
       <c r="D14">
         <v>2010</v>
       </c>
-      <c r="E14" s="2"/>
+      <c r="E14" s="3"/>
       <c r="F14">
         <v>2010</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="1"/>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="2"/>
       <c r="D15">
         <v>2009</v>
       </c>
-      <c r="E15" s="2"/>
+      <c r="E15" s="3"/>
       <c r="F15">
         <v>2009</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="1"/>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="2"/>
       <c r="D16">
         <v>2008</v>
       </c>
-      <c r="E16" s="2"/>
+      <c r="E16" s="3"/>
       <c r="F16">
         <v>2008</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="1"/>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="2"/>
       <c r="D17">
         <v>2007</v>
       </c>
-      <c r="E17" s="2"/>
+      <c r="E17" s="3"/>
       <c r="F17">
         <v>2007</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="1"/>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="2"/>
       <c r="D18">
         <v>2006</v>
       </c>
-      <c r="E18" s="2"/>
+      <c r="E18" s="3"/>
       <c r="F18">
         <v>2006</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="1"/>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="2"/>
       <c r="D19">
         <v>2005</v>
       </c>
-      <c r="E19" s="2"/>
+      <c r="E19" s="3"/>
       <c r="F19">
         <v>2005</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="1"/>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="2"/>
       <c r="D20">
         <v>2004</v>
       </c>
-      <c r="E20" s="2"/>
+      <c r="E20" s="3"/>
       <c r="F20">
         <v>2004</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="1"/>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="2"/>
       <c r="D21">
         <v>2003</v>
       </c>
-      <c r="E21" s="2"/>
+      <c r="E21" s="3"/>
       <c r="F21">
         <v>2003</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="1"/>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="2"/>
       <c r="D22">
         <v>2002</v>
       </c>
-      <c r="E22" s="2"/>
+      <c r="E22" s="3"/>
       <c r="F22">
         <v>2002</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="1"/>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="2"/>
       <c r="D23">
         <v>2001</v>
       </c>
-      <c r="E23" s="2"/>
+      <c r="E23" s="3"/>
       <c r="F23">
         <v>2001</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="1"/>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="2"/>
       <c r="D24">
         <v>2000</v>
       </c>
-      <c r="E24" s="2"/>
+      <c r="E24" s="3"/>
       <c r="F24">
         <v>2000</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="1"/>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="2"/>
       <c r="D25">
         <v>1999</v>
       </c>
-      <c r="E25" s="2"/>
+      <c r="E25" s="3"/>
       <c r="F25">
         <v>1999</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C26" s="1"/>
+      <c r="C26" s="2"/>
       <c r="D26">
         <v>2020</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E26" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F26" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
       <c r="D27">
         <v>2019</v>
       </c>
-      <c r="E27" s="2"/>
+      <c r="E27" s="3"/>
       <c r="F27" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
       <c r="D28">
         <v>2018</v>
       </c>
-      <c r="E28" s="2"/>
+      <c r="E28" s="3"/>
       <c r="F28" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
       <c r="D29">
         <v>2017</v>
       </c>
-      <c r="E29" s="2"/>
+      <c r="E29" s="3"/>
       <c r="F29" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
       <c r="D30">
         <v>2016</v>
       </c>
-      <c r="E30" s="2"/>
+      <c r="E30" s="3"/>
       <c r="F30" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
       <c r="D31">
         <v>2015</v>
       </c>
-      <c r="E31" s="2"/>
+      <c r="E31" s="3"/>
       <c r="F31" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
       <c r="D32">
         <v>2014</v>
       </c>
-      <c r="E32" s="2"/>
+      <c r="E32" s="3"/>
       <c r="F32" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
       <c r="D33">
         <v>2013</v>
       </c>
-      <c r="E33" s="2"/>
+      <c r="E33" s="3"/>
       <c r="F33" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
       <c r="D34">
         <v>2012</v>
       </c>
-      <c r="E34" s="2"/>
+      <c r="E34" s="3"/>
       <c r="F34" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
       <c r="D35">
         <v>2011</v>
       </c>
-      <c r="E35" s="2"/>
+      <c r="E35" s="3"/>
       <c r="F35" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
       <c r="D36">
         <v>2010</v>
       </c>
-      <c r="E36" s="2"/>
+      <c r="E36" s="3"/>
       <c r="F36" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
       <c r="D37">
         <v>2009</v>
       </c>
-      <c r="E37" s="2"/>
+      <c r="E37" s="3"/>
       <c r="F37" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
       <c r="D38">
         <v>2008</v>
       </c>
-      <c r="E38" s="2"/>
+      <c r="E38" s="3"/>
       <c r="F38" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
       <c r="D39">
         <v>2007</v>
       </c>
-      <c r="E39" s="2"/>
+      <c r="E39" s="3"/>
       <c r="F39" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
       <c r="D40">
         <v>2006</v>
       </c>
-      <c r="E40" s="2"/>
+      <c r="E40" s="3"/>
       <c r="F40" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
       <c r="D41">
         <v>2005</v>
       </c>
-      <c r="E41" s="2"/>
+      <c r="E41" s="3"/>
       <c r="F41" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
       <c r="D42">
         <v>2004</v>
       </c>
-      <c r="E42" s="2"/>
+      <c r="E42" s="3"/>
       <c r="F42" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
       <c r="D43">
         <v>2003</v>
       </c>
-      <c r="E43" s="2"/>
+      <c r="E43" s="3"/>
       <c r="F43" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
-      <c r="B44" s="1" t="s">
+      <c r="B44" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C44" s="1"/>
+      <c r="C44" s="2"/>
       <c r="D44">
         <v>2020</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="E44" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F44" t="s">
         <v>50</v>
       </c>
-      <c r="H44" s="2" t="s">
+      <c r="H44" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
       <c r="D45">
         <v>2019</v>
       </c>
-      <c r="E45" s="2"/>
+      <c r="E45" s="3"/>
       <c r="F45" t="s">
         <v>35</v>
       </c>
-      <c r="H45" s="2"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H45" s="3"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
       <c r="D46">
         <v>2018</v>
       </c>
-      <c r="E46" s="2"/>
+      <c r="E46" s="3"/>
       <c r="F46" t="s">
         <v>36</v>
       </c>
-      <c r="H46" s="2"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H46" s="3"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
       <c r="D47">
         <v>2017</v>
       </c>
-      <c r="E47" s="2"/>
+      <c r="E47" s="3"/>
       <c r="F47" t="s">
         <v>37</v>
       </c>
-      <c r="H47" s="2"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H47" s="3"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
       <c r="D48">
         <v>2016</v>
       </c>
-      <c r="E48" s="2"/>
+      <c r="E48" s="3"/>
       <c r="F48" t="s">
         <v>38</v>
       </c>
-      <c r="H48" s="2"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H48" s="3"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
       <c r="D49">
         <v>2015</v>
       </c>
-      <c r="E49" s="2"/>
+      <c r="E49" s="3"/>
       <c r="F49" t="s">
         <v>39</v>
       </c>
-      <c r="H49" s="2"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H49" s="3"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
       <c r="D50">
         <v>2014</v>
       </c>
-      <c r="E50" s="2"/>
+      <c r="E50" s="3"/>
       <c r="F50" t="s">
         <v>40</v>
       </c>
-      <c r="H50" s="2"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H50" s="3"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
       <c r="D51">
         <v>2013</v>
       </c>
-      <c r="E51" s="2"/>
+      <c r="E51" s="3"/>
       <c r="F51" t="s">
         <v>41</v>
       </c>
-      <c r="H51" s="2"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H51" s="3"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
       <c r="D52">
         <v>2012</v>
       </c>
-      <c r="E52" s="2"/>
+      <c r="E52" s="3"/>
       <c r="F52" t="s">
         <v>42</v>
       </c>
-      <c r="H52" s="2"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H52" s="3"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
       <c r="D53">
         <v>2011</v>
       </c>
-      <c r="E53" s="2"/>
+      <c r="E53" s="3"/>
       <c r="F53" t="s">
         <v>43</v>
       </c>
-      <c r="H53" s="2"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H53" s="3"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
       <c r="D54">
         <v>2010</v>
       </c>
-      <c r="E54" s="2"/>
+      <c r="E54" s="3"/>
       <c r="F54" t="s">
         <v>44</v>
       </c>
-      <c r="H54" s="2"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H54" s="3"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
       <c r="D55">
         <v>2009</v>
       </c>
-      <c r="E55" s="2"/>
+      <c r="E55" s="3"/>
       <c r="F55" t="s">
         <v>45</v>
       </c>
-      <c r="H55" s="2"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H55" s="3"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
       <c r="D56">
         <v>2008</v>
       </c>
-      <c r="E56" s="2"/>
+      <c r="E56" s="3"/>
       <c r="F56" t="s">
         <v>46</v>
       </c>
-      <c r="H56" s="2"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H56" s="3"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
       <c r="D57">
         <v>2007</v>
       </c>
-      <c r="E57" s="2"/>
+      <c r="E57" s="3"/>
       <c r="F57" t="s">
         <v>47</v>
       </c>
-      <c r="H57" s="2"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H57" s="3"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
       <c r="D58">
         <v>2006</v>
       </c>
-      <c r="E58" s="2"/>
+      <c r="E58" s="3"/>
       <c r="F58" t="s">
         <v>48</v>
       </c>
-      <c r="H58" s="2"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H58" s="3"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
       <c r="D59">
         <v>2005</v>
       </c>
-      <c r="E59" s="2"/>
+      <c r="E59" s="3"/>
       <c r="F59" t="s">
         <v>49</v>
       </c>
-      <c r="H59" s="2"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H59" s="3"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
       <c r="D60">
         <v>2004</v>
       </c>
-      <c r="E60" s="2"/>
+      <c r="E60" s="3"/>
       <c r="F60" t="s">
         <v>34</v>
       </c>
-      <c r="H60" s="2"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H60" s="3"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
       <c r="D61">
         <v>2003</v>
       </c>
-      <c r="E61" s="2"/>
+      <c r="E61" s="3"/>
       <c r="F61" t="s">
         <v>33</v>
       </c>
-      <c r="H61" s="2"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H61" s="3"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
-      <c r="B62" s="1" t="s">
+      <c r="B62" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C62" s="1"/>
+      <c r="C62" s="2"/>
       <c r="D62">
         <v>2020</v>
       </c>
-      <c r="E62" s="3" t="s">
+      <c r="E62" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F62" t="s">
         <v>51</v>
       </c>
-      <c r="H62" s="2" t="s">
+      <c r="H62" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
       <c r="D63">
         <v>2019</v>
       </c>
-      <c r="E63" s="2"/>
+      <c r="E63" s="3"/>
       <c r="F63" t="s">
         <v>52</v>
       </c>
-      <c r="H63" s="2"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H63" s="3"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
-      <c r="B64" s="1"/>
-      <c r="C64" s="1"/>
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
       <c r="D64">
         <v>2018</v>
       </c>
-      <c r="E64" s="2"/>
+      <c r="E64" s="3"/>
       <c r="F64" t="s">
         <v>53</v>
       </c>
-      <c r="H64" s="2"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H64" s="3"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
       <c r="D65">
         <v>2017</v>
       </c>
-      <c r="E65" s="2"/>
+      <c r="E65" s="3"/>
       <c r="F65" t="s">
         <v>54</v>
       </c>
-      <c r="H65" s="2"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H65" s="3"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="4"/>
-      <c r="B66" s="1"/>
-      <c r="C66" s="1"/>
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
       <c r="D66">
         <v>2016</v>
       </c>
-      <c r="E66" s="2"/>
+      <c r="E66" s="3"/>
       <c r="F66" t="s">
         <v>55</v>
       </c>
-      <c r="H66" s="2"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H66" s="3"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="4"/>
-      <c r="B67" s="1"/>
-      <c r="C67" s="1"/>
+      <c r="B67" s="2"/>
+      <c r="C67" s="2"/>
       <c r="D67">
         <v>2015</v>
       </c>
-      <c r="E67" s="2"/>
+      <c r="E67" s="3"/>
       <c r="F67" t="s">
         <v>56</v>
       </c>
-      <c r="H67" s="2"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H67" s="3"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="4"/>
-      <c r="B68" s="1"/>
-      <c r="C68" s="1"/>
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
       <c r="D68">
         <v>2014</v>
       </c>
-      <c r="E68" s="2"/>
+      <c r="E68" s="3"/>
       <c r="F68" t="s">
         <v>57</v>
       </c>
-      <c r="H68" s="2"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H68" s="3"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="4"/>
-      <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
+      <c r="B69" s="2"/>
+      <c r="C69" s="2"/>
       <c r="D69">
         <v>2013</v>
       </c>
-      <c r="E69" s="2"/>
+      <c r="E69" s="3"/>
       <c r="F69" t="s">
         <v>58</v>
       </c>
-      <c r="H69" s="2"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H69" s="3"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="4"/>
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
+      <c r="B70" s="2"/>
+      <c r="C70" s="2"/>
       <c r="D70">
         <v>2012</v>
       </c>
-      <c r="E70" s="2"/>
+      <c r="E70" s="3"/>
       <c r="F70" t="s">
         <v>59</v>
       </c>
-      <c r="H70" s="2"/>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H70" s="3"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="4"/>
-      <c r="B71" s="1"/>
-      <c r="C71" s="1"/>
+      <c r="B71" s="2"/>
+      <c r="C71" s="2"/>
       <c r="D71">
         <v>2011</v>
       </c>
-      <c r="E71" s="2"/>
+      <c r="E71" s="3"/>
       <c r="F71" t="s">
         <v>60</v>
       </c>
-      <c r="H71" s="2"/>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H71" s="3"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="4"/>
-      <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
+      <c r="B72" s="2"/>
+      <c r="C72" s="2"/>
       <c r="D72">
         <v>2010</v>
       </c>
-      <c r="E72" s="2"/>
+      <c r="E72" s="3"/>
       <c r="F72" t="s">
         <v>61</v>
       </c>
-      <c r="H72" s="2"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H72" s="3"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
-      <c r="B73" s="1"/>
-      <c r="C73" s="1"/>
+      <c r="B73" s="2"/>
+      <c r="C73" s="2"/>
       <c r="D73">
         <v>2009</v>
       </c>
-      <c r="E73" s="2"/>
+      <c r="E73" s="3"/>
       <c r="F73" t="s">
         <v>62</v>
       </c>
-      <c r="H73" s="2"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H73" s="3"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
-      <c r="B74" s="1"/>
-      <c r="C74" s="1"/>
+      <c r="B74" s="2"/>
+      <c r="C74" s="2"/>
       <c r="D74">
         <v>2008</v>
       </c>
-      <c r="E74" s="2"/>
+      <c r="E74" s="3"/>
       <c r="F74" t="s">
         <v>63</v>
       </c>
-      <c r="H74" s="2"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H74" s="3"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="4"/>
-      <c r="B75" s="1"/>
-      <c r="C75" s="1"/>
+      <c r="B75" s="2"/>
+      <c r="C75" s="2"/>
       <c r="D75">
         <v>2007</v>
       </c>
-      <c r="E75" s="2"/>
+      <c r="E75" s="3"/>
       <c r="F75" t="s">
         <v>64</v>
       </c>
-      <c r="H75" s="2"/>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H75" s="3"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="4"/>
-      <c r="B76" s="1"/>
-      <c r="C76" s="1"/>
+      <c r="B76" s="2"/>
+      <c r="C76" s="2"/>
       <c r="D76">
         <v>2006</v>
       </c>
-      <c r="E76" s="2"/>
+      <c r="E76" s="3"/>
       <c r="F76" t="s">
         <v>65</v>
       </c>
-      <c r="H76" s="2"/>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H76" s="3"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="4"/>
-      <c r="B77" s="1"/>
-      <c r="C77" s="1"/>
+      <c r="B77" s="2"/>
+      <c r="C77" s="2"/>
       <c r="D77">
         <v>2005</v>
       </c>
-      <c r="E77" s="2"/>
+      <c r="E77" s="3"/>
       <c r="F77" t="s">
         <v>66</v>
       </c>
-      <c r="H77" s="2"/>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H77" s="3"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
-      <c r="B78" s="1"/>
-      <c r="C78" s="1"/>
+      <c r="B78" s="2"/>
+      <c r="C78" s="2"/>
       <c r="D78">
         <v>2004</v>
       </c>
-      <c r="E78" s="2"/>
+      <c r="E78" s="3"/>
       <c r="F78" t="s">
         <v>67</v>
       </c>
-      <c r="H78" s="2"/>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H78" s="3"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="4"/>
-      <c r="B79" s="1"/>
-      <c r="C79" s="1"/>
+      <c r="B79" s="2"/>
+      <c r="C79" s="2"/>
       <c r="D79">
         <v>2003</v>
       </c>
-      <c r="E79" s="2"/>
+      <c r="E79" s="3"/>
       <c r="F79" t="s">
         <v>68</v>
       </c>
-      <c r="H79" s="2"/>
-    </row>
-    <row r="80" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H79" s="3"/>
+    </row>
+    <row r="80" spans="1:8" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="C80" s="1"/>
-      <c r="E80" s="2" t="s">
+      <c r="C80" s="7"/>
+      <c r="D80" s="6"/>
+      <c r="E80" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="F80" t="s">
+      <c r="F80" s="6" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="4"/>
-      <c r="B81" t="s">
+      <c r="B81" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="C81" s="1"/>
-      <c r="E81" s="2"/>
-      <c r="F81" t="s">
+      <c r="C81" s="7"/>
+      <c r="D81" s="6"/>
+      <c r="E81" s="8"/>
+      <c r="F81" s="6" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="4"/>
-      <c r="B82" t="s">
+      <c r="B82" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="C82" s="1"/>
-      <c r="E82" s="2"/>
-      <c r="F82" t="s">
+      <c r="C82" s="7"/>
+      <c r="D82" s="6"/>
+      <c r="E82" s="8"/>
+      <c r="F82" s="6" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
-      <c r="B83" t="s">
+      <c r="B83" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="C83" s="1"/>
-      <c r="E83" s="2"/>
-      <c r="F83" t="s">
+      <c r="C83" s="7"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="8"/>
+      <c r="F83" s="6" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
-      <c r="B84" t="s">
+      <c r="B84" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="C84" s="1"/>
-      <c r="E84" s="2"/>
-      <c r="F84" t="s">
+      <c r="C84" s="7"/>
+      <c r="D84" s="6"/>
+      <c r="E84" s="8"/>
+      <c r="F84" s="6" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="4"/>
-      <c r="B85" t="s">
+      <c r="B85" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="C85" s="1"/>
-      <c r="E85" s="2"/>
-      <c r="F85" t="s">
+      <c r="C85" s="7"/>
+      <c r="D85" s="6"/>
+      <c r="E85" s="8"/>
+      <c r="F85" s="6" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="4"/>
-      <c r="B86" t="s">
+      <c r="B86" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="C86" s="1"/>
-      <c r="E86" s="2"/>
-      <c r="F86" t="s">
+      <c r="C86" s="7"/>
+      <c r="D86" s="6"/>
+      <c r="E86" s="8"/>
+      <c r="F86" s="6" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="4"/>
-      <c r="B87" t="s">
+      <c r="B87" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="C87" s="1"/>
-      <c r="E87" s="2"/>
-      <c r="F87" t="s">
+      <c r="C87" s="7"/>
+      <c r="D87" s="6"/>
+      <c r="E87" s="8"/>
+      <c r="F87" s="6" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="4"/>
-      <c r="B88" t="s">
+      <c r="B88" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="C88" s="1"/>
-      <c r="E88" s="2"/>
-      <c r="F88" t="s">
+      <c r="C88" s="7"/>
+      <c r="D88" s="6"/>
+      <c r="E88" s="8"/>
+      <c r="F88" s="6" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="4"/>
-      <c r="B89" t="s">
+      <c r="B89" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="C89" s="1"/>
-      <c r="E89" s="2"/>
-      <c r="F89" t="s">
+      <c r="C89" s="7"/>
+      <c r="D89" s="6"/>
+      <c r="E89" s="8"/>
+      <c r="F89" s="6" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="4"/>
-      <c r="B90" t="s">
+      <c r="B90" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="C90" s="1"/>
-      <c r="E90" s="2"/>
-      <c r="F90" t="s">
+      <c r="C90" s="7"/>
+      <c r="D90" s="6"/>
+      <c r="E90" s="8"/>
+      <c r="F90" s="6" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="4"/>
-      <c r="B91" t="s">
+      <c r="B91" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="C91" s="1"/>
-      <c r="E91" s="2"/>
-      <c r="F91" t="s">
+      <c r="C91" s="7"/>
+      <c r="D91" s="6"/>
+      <c r="E91" s="8"/>
+      <c r="F91" s="6" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="4"/>
-      <c r="B92" t="s">
+      <c r="B92" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C92" s="1"/>
-      <c r="E92" s="2"/>
-      <c r="F92" t="s">
+      <c r="C92" s="7"/>
+      <c r="D92" s="6"/>
+      <c r="E92" s="8"/>
+      <c r="F92" s="6" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="4"/>
-      <c r="B93" t="s">
+      <c r="B93" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="C93" s="1"/>
-      <c r="E93" s="2"/>
-      <c r="F93" t="s">
+      <c r="C93" s="7"/>
+      <c r="D93" s="6"/>
+      <c r="E93" s="8"/>
+      <c r="F93" s="6" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="4"/>
-      <c r="B94" t="s">
+      <c r="B94" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="C94" s="1"/>
-      <c r="E94" s="2"/>
-      <c r="F94" t="s">
+      <c r="C94" s="7"/>
+      <c r="D94" s="6"/>
+      <c r="E94" s="8"/>
+      <c r="F94" s="6" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="4"/>
-      <c r="B95" t="s">
+      <c r="B95" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="C95" s="1"/>
-      <c r="E95" s="2"/>
-      <c r="F95" t="s">
+      <c r="C95" s="7"/>
+      <c r="D95" s="6"/>
+      <c r="E95" s="8"/>
+      <c r="F95" s="6" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="4"/>
-      <c r="B96" t="s">
+      <c r="B96" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="C96" s="1"/>
-      <c r="E96" s="2"/>
-      <c r="F96" t="s">
+      <c r="C96" s="7"/>
+      <c r="D96" s="6"/>
+      <c r="E96" s="8"/>
+      <c r="F96" s="6" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="4"/>
-      <c r="B97" t="s">
+      <c r="B97" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="C97" s="1"/>
-      <c r="E97" s="2"/>
-      <c r="F97" t="s">
+      <c r="C97" s="7"/>
+      <c r="D97" s="6"/>
+      <c r="E97" s="8"/>
+      <c r="F97" s="6" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="4"/>
-      <c r="B98" t="s">
+      <c r="B98" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="C98" s="1"/>
-      <c r="E98" s="2"/>
-      <c r="F98" t="s">
+      <c r="C98" s="7"/>
+      <c r="D98" s="6"/>
+      <c r="E98" s="8"/>
+      <c r="F98" s="6" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="4"/>
-      <c r="B99" t="s">
+      <c r="B99" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="C99" s="1"/>
-      <c r="E99" s="2"/>
-      <c r="F99" t="s">
+      <c r="C99" s="7"/>
+      <c r="D99" s="6"/>
+      <c r="E99" s="8"/>
+      <c r="F99" s="6" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="4"/>
-      <c r="B100" t="s">
+      <c r="B100" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="C100" s="1"/>
-      <c r="E100" s="2"/>
-      <c r="F100" t="s">
+      <c r="C100" s="7"/>
+      <c r="D100" s="6"/>
+      <c r="E100" s="8"/>
+      <c r="F100" s="6" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="4"/>
-      <c r="B101" t="s">
+      <c r="B101" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C101" s="1"/>
-      <c r="E101" s="2"/>
-      <c r="H101" s="2" t="s">
+      <c r="C101" s="7"/>
+      <c r="D101" s="6"/>
+      <c r="E101" s="8"/>
+      <c r="F101" s="6"/>
+      <c r="H101" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="4"/>
-      <c r="B102" t="s">
+      <c r="B102" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C102" s="1"/>
-      <c r="E102" s="2"/>
-      <c r="H102" s="2"/>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C102" s="7"/>
+      <c r="D102" s="6"/>
+      <c r="E102" s="8"/>
+      <c r="F102" s="6"/>
+      <c r="H102" s="3"/>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="4"/>
-      <c r="B103" t="s">
+      <c r="B103" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C103" s="6" t="s">
+      <c r="C103" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="E103" s="2"/>
-      <c r="H103" s="2"/>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D103" s="6"/>
+      <c r="E103" s="8"/>
+      <c r="F103" s="6"/>
+      <c r="H103" s="3"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="4"/>
-      <c r="B104" t="s">
+      <c r="B104" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="C104" s="6"/>
-      <c r="E104" s="2"/>
-      <c r="H104" s="2"/>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C104" s="9"/>
+      <c r="D104" s="6"/>
+      <c r="E104" s="8"/>
+      <c r="F104" s="6"/>
+      <c r="H104" s="3"/>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="4"/>
-      <c r="B105" t="s">
+      <c r="B105" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="C105" s="1"/>
-      <c r="E105" s="2"/>
-      <c r="H105" s="2"/>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C105" s="7"/>
+      <c r="D105" s="6"/>
+      <c r="E105" s="8"/>
+      <c r="F105" s="6"/>
+      <c r="H105" s="3"/>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="4"/>
-      <c r="B106" t="s">
+      <c r="B106" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C106" s="1"/>
-      <c r="E106" s="2"/>
-      <c r="H106" s="2"/>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C106" s="7"/>
+      <c r="D106" s="6"/>
+      <c r="E106" s="8"/>
+      <c r="F106" s="6"/>
+      <c r="H106" s="3"/>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="4"/>
-      <c r="B107" t="s">
+      <c r="B107" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="C107" s="1"/>
-      <c r="E107" s="2"/>
-      <c r="H107" s="2"/>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C107" s="7"/>
+      <c r="D107" s="6"/>
+      <c r="E107" s="8"/>
+      <c r="F107" s="6"/>
+      <c r="H107" s="3"/>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="4"/>
-      <c r="B108" t="s">
+      <c r="B108" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C108" s="1"/>
-      <c r="E108" s="2"/>
-      <c r="H108" s="2"/>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C108" s="7"/>
+      <c r="D108" s="6"/>
+      <c r="E108" s="8"/>
+      <c r="F108" s="6"/>
+      <c r="H108" s="3"/>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="4"/>
-      <c r="B109" t="s">
+      <c r="B109" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="C109" s="1"/>
-      <c r="E109" s="2"/>
-      <c r="H109" s="2"/>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C109" s="7"/>
+      <c r="D109" s="6"/>
+      <c r="E109" s="8"/>
+      <c r="F109" s="6"/>
+      <c r="H109" s="3"/>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="4"/>
-      <c r="B110" t="s">
+      <c r="B110" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="C110" s="1"/>
-      <c r="E110" s="2"/>
-      <c r="H110" s="2"/>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C110" s="7"/>
+      <c r="D110" s="6"/>
+      <c r="E110" s="8"/>
+      <c r="F110" s="6"/>
+      <c r="H110" s="3"/>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="4"/>
-      <c r="B111" t="s">
+      <c r="B111" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="C111" s="1"/>
-      <c r="E111" s="2"/>
-      <c r="H111" s="2"/>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C111" s="7"/>
+      <c r="D111" s="6"/>
+      <c r="E111" s="8"/>
+      <c r="F111" s="6"/>
+      <c r="H111" s="3"/>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="4"/>
-      <c r="B112" t="s">
+      <c r="B112" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="C112" s="1"/>
-      <c r="E112" s="2"/>
-      <c r="H112" s="2"/>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C112" s="7"/>
+      <c r="D112" s="6"/>
+      <c r="E112" s="8"/>
+      <c r="F112" s="6"/>
+      <c r="H112" s="3"/>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="4"/>
-      <c r="B113" t="s">
+      <c r="B113" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C113" s="1"/>
-      <c r="E113" s="2"/>
-      <c r="H113" s="2"/>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C113" s="7"/>
+      <c r="D113" s="6"/>
+      <c r="E113" s="8"/>
+      <c r="F113" s="6"/>
+      <c r="H113" s="3"/>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="4"/>
-      <c r="B114" t="s">
+      <c r="B114" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="C114" s="1"/>
-      <c r="E114" s="2"/>
-      <c r="H114" s="2"/>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C114" s="7"/>
+      <c r="D114" s="6"/>
+      <c r="E114" s="8"/>
+      <c r="F114" s="6"/>
+      <c r="H114" s="3"/>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="4"/>
-      <c r="B115" t="s">
+      <c r="B115" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="C115" s="1"/>
-      <c r="E115" s="2"/>
-      <c r="H115" s="2"/>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C115" s="7"/>
+      <c r="D115" s="6"/>
+      <c r="E115" s="8"/>
+      <c r="F115" s="6"/>
+      <c r="H115" s="3"/>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="4"/>
-      <c r="B116" t="s">
+      <c r="B116" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="C116" s="1"/>
-      <c r="E116" s="2"/>
-      <c r="H116" s="2"/>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C116" s="7"/>
+      <c r="D116" s="6"/>
+      <c r="E116" s="8"/>
+      <c r="F116" s="6"/>
+      <c r="H116" s="3"/>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="4"/>
-      <c r="B117" t="s">
+      <c r="B117" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C117" s="1"/>
-      <c r="E117" s="2"/>
-      <c r="H117" s="2"/>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C117" s="7"/>
+      <c r="D117" s="6"/>
+      <c r="E117" s="8"/>
+      <c r="F117" s="6"/>
+      <c r="H117" s="3"/>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="4"/>
-      <c r="B118" t="s">
+      <c r="B118" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="C118" s="1"/>
-      <c r="E118" s="2"/>
-      <c r="H118" s="2"/>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C118" s="7"/>
+      <c r="D118" s="6"/>
+      <c r="E118" s="8"/>
+      <c r="F118" s="6"/>
+      <c r="H118" s="3"/>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="4"/>
-      <c r="B119" t="s">
+      <c r="B119" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="C119" s="1"/>
-      <c r="E119" s="2"/>
-      <c r="H119" s="2"/>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C119" s="7"/>
+      <c r="D119" s="6"/>
+      <c r="E119" s="8"/>
+      <c r="F119" s="6"/>
+      <c r="H119" s="3"/>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>119</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B120" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="D120">
+      <c r="C120" s="6"/>
+      <c r="D120" s="6">
         <v>2011</v>
       </c>
-      <c r="E120" s="2"/>
-      <c r="F120" t="s">
+      <c r="E120" s="8"/>
+      <c r="F120" s="6" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="121" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="2" t="s">
+    <row r="121" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="3" t="s">
         <v>143</v>
       </c>
       <c r="B121" t="s">
         <v>144</v>
       </c>
-      <c r="C121" s="5"/>
-      <c r="D121" s="1">
+      <c r="C121" s="1"/>
+      <c r="D121" s="2">
         <v>2017</v>
       </c>
-      <c r="E121" s="2" t="s">
+      <c r="E121" s="3" t="s">
         <v>150</v>
       </c>
       <c r="F121" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A122" s="2"/>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A122" s="3"/>
       <c r="B122" t="s">
         <v>145</v>
       </c>
-      <c r="C122" s="5"/>
-      <c r="D122" s="1"/>
-      <c r="E122" s="2"/>
+      <c r="C122" s="1"/>
+      <c r="D122" s="2"/>
+      <c r="E122" s="3"/>
       <c r="F122" t="s">
         <v>148</v>
       </c>
@@ -2393,40 +2460,40 @@
         <v>151</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A123" s="2"/>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A123" s="3"/>
       <c r="B123" t="s">
         <v>146</v>
       </c>
-      <c r="C123" s="5"/>
-      <c r="D123" s="1"/>
-      <c r="E123" s="2"/>
+      <c r="C123" s="1"/>
+      <c r="D123" s="2"/>
+      <c r="E123" s="3"/>
       <c r="F123" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A124" s="2"/>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A124" s="3"/>
       <c r="B124" t="s">
         <v>152</v>
       </c>
-      <c r="D124" s="1">
+      <c r="D124" s="2">
         <v>2015</v>
       </c>
-      <c r="E124" s="2" t="s">
+      <c r="E124" s="3" t="s">
         <v>154</v>
       </c>
       <c r="F124" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A125" s="2"/>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A125" s="3"/>
       <c r="B125" t="s">
         <v>153</v>
       </c>
-      <c r="D125" s="1"/>
-      <c r="E125" s="2"/>
+      <c r="D125" s="2"/>
+      <c r="E125" s="3"/>
       <c r="F125" t="s">
         <v>148</v>
       </c>
@@ -2434,12 +2501,12 @@
         <v>151</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A126" s="2"/>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A126" s="3"/>
       <c r="B126" t="s">
         <v>157</v>
       </c>
-      <c r="D126" s="1"/>
+      <c r="D126" s="2"/>
       <c r="E126" t="s">
         <v>155</v>
       </c>
@@ -2447,15 +2514,15 @@
         <v>156</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A127" s="2"/>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A127" s="3"/>
       <c r="B127" t="s">
         <v>159</v>
       </c>
-      <c r="D127" s="1">
+      <c r="D127" s="2">
         <v>2013</v>
       </c>
-      <c r="E127" s="1" t="s">
+      <c r="E127" s="2" t="s">
         <v>161</v>
       </c>
       <c r="F127" t="s">
@@ -2465,26 +2532,26 @@
         <v>162</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A128" s="2"/>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A128" s="3"/>
       <c r="B128" t="s">
         <v>160</v>
       </c>
-      <c r="D128" s="1"/>
-      <c r="E128" s="1"/>
+      <c r="D128" s="2"/>
+      <c r="E128" s="2"/>
       <c r="F128" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A129" s="2"/>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A129" s="3"/>
       <c r="B129" t="s">
         <v>158</v>
       </c>
-      <c r="D129" s="1">
+      <c r="D129" s="2">
         <v>2008</v>
       </c>
-      <c r="E129" s="1" t="s">
+      <c r="E129" s="2" t="s">
         <v>163</v>
       </c>
       <c r="F129" t="s">
@@ -2494,24 +2561,52 @@
         <v>166</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A130" s="2"/>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A130" s="3"/>
       <c r="B130" t="s">
         <v>165</v>
       </c>
-      <c r="D130" s="1"/>
-      <c r="E130" s="1"/>
+      <c r="D130" s="2"/>
+      <c r="E130" s="2"/>
       <c r="F130" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A131" s="2"/>
-      <c r="D131" s="5"/>
-      <c r="E131" s="5"/>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A131" s="3"/>
+      <c r="D131" s="1"/>
+      <c r="E131" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="A80:A119"/>
+    <mergeCell ref="E80:E120"/>
+    <mergeCell ref="E44:E61"/>
+    <mergeCell ref="B44:B61"/>
+    <mergeCell ref="C44:C61"/>
+    <mergeCell ref="B62:B79"/>
+    <mergeCell ref="C62:C79"/>
+    <mergeCell ref="E62:E79"/>
+    <mergeCell ref="H44:H61"/>
+    <mergeCell ref="H62:H79"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A25"/>
+    <mergeCell ref="A26:A79"/>
+    <mergeCell ref="B5:B25"/>
+    <mergeCell ref="E5:E25"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B26:B43"/>
+    <mergeCell ref="C26:C43"/>
+    <mergeCell ref="C5:C25"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="E26:E43"/>
+    <mergeCell ref="C103:C104"/>
+    <mergeCell ref="C105:C112"/>
+    <mergeCell ref="C113:C119"/>
+    <mergeCell ref="H101:H119"/>
+    <mergeCell ref="C80:C86"/>
+    <mergeCell ref="C87:C100"/>
+    <mergeCell ref="C101:C102"/>
     <mergeCell ref="E127:E128"/>
     <mergeCell ref="E129:E130"/>
     <mergeCell ref="A121:A131"/>
@@ -2521,34 +2616,6 @@
     <mergeCell ref="E124:E125"/>
     <mergeCell ref="D127:D128"/>
     <mergeCell ref="D129:D130"/>
-    <mergeCell ref="C103:C104"/>
-    <mergeCell ref="C105:C112"/>
-    <mergeCell ref="C113:C119"/>
-    <mergeCell ref="H101:H119"/>
-    <mergeCell ref="C80:C86"/>
-    <mergeCell ref="C87:C100"/>
-    <mergeCell ref="H44:H61"/>
-    <mergeCell ref="H62:H79"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A25"/>
-    <mergeCell ref="A26:A79"/>
-    <mergeCell ref="C101:C102"/>
-    <mergeCell ref="A80:A119"/>
-    <mergeCell ref="E80:E120"/>
-    <mergeCell ref="E44:E61"/>
-    <mergeCell ref="B44:B61"/>
-    <mergeCell ref="C44:C61"/>
-    <mergeCell ref="B62:B79"/>
-    <mergeCell ref="C62:C79"/>
-    <mergeCell ref="E62:E79"/>
-    <mergeCell ref="B5:B25"/>
-    <mergeCell ref="E5:E25"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B26:B43"/>
-    <mergeCell ref="C26:C43"/>
-    <mergeCell ref="C5:C25"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="E26:E43"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
add 2020. add ditcionary file. fix linkage city type to city name
</commit_message>
<xml_diff>
--- a/originals/files catalog.xlsx
+++ b/originals/files catalog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OWNER\Dropbox\projects\local_authorities_in_Israel\originals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4517E3F4-D254-4BD9-B779-6370F51180F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C07471A-7AF7-4A02-9A58-4B31EE4BC106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="172">
   <si>
     <t>שם הקובץ</t>
   </si>
@@ -541,6 +541,15 @@
   </si>
   <si>
     <t>רחובות עיקריים ושכונות לאס</t>
+  </si>
+  <si>
+    <t>לא השתמשתי. ניתן להוסיף בעתיד אם הלמס תמשיך לפרסם טבלה זו</t>
+  </si>
+  <si>
+    <t>population_madaf_2020_9</t>
+  </si>
+  <si>
+    <t>אוכלוסייה לפי צורת יישוב, יישוב, אזור סטטיסטי, מין וגיל, סוף 2020</t>
   </si>
 </sst>
 </file>
@@ -601,27 +610,27 @@
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -904,16 +913,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H131"/>
+  <dimension ref="A1:H132"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F84" sqref="F84"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I94" sqref="I94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="57.28515625" customWidth="1"/>
+    <col min="2" max="2" width="77.7109375" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.28515625" customWidth="1"/>
     <col min="6" max="6" width="29.140625" customWidth="1"/>
@@ -946,13 +955,13 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="7"/>
       <c r="D2">
         <v>2019</v>
       </c>
@@ -961,9 +970,9 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
       <c r="D3">
         <v>2018</v>
       </c>
@@ -972,9 +981,9 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
       <c r="D4">
         <v>2017</v>
       </c>
@@ -983,17 +992,17 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="7"/>
       <c r="D5">
         <v>2019</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="6" t="s">
         <v>72</v>
       </c>
       <c r="F5">
@@ -1001,253 +1010,253 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="2"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="7"/>
       <c r="D6">
         <v>2018</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="E6" s="6"/>
       <c r="F6">
         <v>2018</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="2"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="7"/>
       <c r="D7">
         <v>2017</v>
       </c>
-      <c r="E7" s="3"/>
+      <c r="E7" s="6"/>
       <c r="F7">
         <v>2017</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="2"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="7"/>
       <c r="D8">
         <v>2016</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="6"/>
       <c r="F8">
         <v>2016</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="2"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="7"/>
       <c r="D9">
         <v>2015</v>
       </c>
-      <c r="E9" s="3"/>
+      <c r="E9" s="6"/>
       <c r="F9">
         <v>2015</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="2"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="7"/>
       <c r="D10">
         <v>2014</v>
       </c>
-      <c r="E10" s="3"/>
+      <c r="E10" s="6"/>
       <c r="F10">
         <v>2014</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="2"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="7"/>
       <c r="D11">
         <v>2013</v>
       </c>
-      <c r="E11" s="3"/>
+      <c r="E11" s="6"/>
       <c r="F11">
         <v>2013</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="2"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="7"/>
       <c r="D12">
         <v>2012</v>
       </c>
-      <c r="E12" s="3"/>
+      <c r="E12" s="6"/>
       <c r="F12">
         <v>2012</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="2"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="7"/>
       <c r="D13">
         <v>2011</v>
       </c>
-      <c r="E13" s="3"/>
+      <c r="E13" s="6"/>
       <c r="F13">
         <v>2011</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="2"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="7"/>
       <c r="D14">
         <v>2010</v>
       </c>
-      <c r="E14" s="3"/>
+      <c r="E14" s="6"/>
       <c r="F14">
         <v>2010</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="2"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="7"/>
       <c r="D15">
         <v>2009</v>
       </c>
-      <c r="E15" s="3"/>
+      <c r="E15" s="6"/>
       <c r="F15">
         <v>2009</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="2"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="7"/>
       <c r="D16">
         <v>2008</v>
       </c>
-      <c r="E16" s="3"/>
+      <c r="E16" s="6"/>
       <c r="F16">
         <v>2008</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="2"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="7"/>
       <c r="D17">
         <v>2007</v>
       </c>
-      <c r="E17" s="3"/>
+      <c r="E17" s="6"/>
       <c r="F17">
         <v>2007</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="2"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="7"/>
       <c r="D18">
         <v>2006</v>
       </c>
-      <c r="E18" s="3"/>
+      <c r="E18" s="6"/>
       <c r="F18">
         <v>2006</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="2"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="7"/>
       <c r="D19">
         <v>2005</v>
       </c>
-      <c r="E19" s="3"/>
+      <c r="E19" s="6"/>
       <c r="F19">
         <v>2005</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="2"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="7"/>
       <c r="D20">
         <v>2004</v>
       </c>
-      <c r="E20" s="3"/>
+      <c r="E20" s="6"/>
       <c r="F20">
         <v>2004</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="2"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="7"/>
       <c r="D21">
         <v>2003</v>
       </c>
-      <c r="E21" s="3"/>
+      <c r="E21" s="6"/>
       <c r="F21">
         <v>2003</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="2"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="7"/>
       <c r="D22">
         <v>2002</v>
       </c>
-      <c r="E22" s="3"/>
+      <c r="E22" s="6"/>
       <c r="F22">
         <v>2002</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="2"/>
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="7"/>
       <c r="D23">
         <v>2001</v>
       </c>
-      <c r="E23" s="3"/>
+      <c r="E23" s="6"/>
       <c r="F23">
         <v>2001</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="2"/>
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="7"/>
       <c r="D24">
         <v>2000</v>
       </c>
-      <c r="E24" s="3"/>
+      <c r="E24" s="6"/>
       <c r="F24">
         <v>2000</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="2"/>
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="7"/>
       <c r="D25">
         <v>1999</v>
       </c>
-      <c r="E25" s="3"/>
+      <c r="E25" s="6"/>
       <c r="F25">
         <v>1999</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C26" s="2"/>
+      <c r="C26" s="7"/>
       <c r="D26">
         <v>2020</v>
       </c>
@@ -1259,215 +1268,215 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
+      <c r="A27" s="3"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
       <c r="D27">
         <v>2019</v>
       </c>
-      <c r="E27" s="3"/>
+      <c r="E27" s="6"/>
       <c r="F27" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
+      <c r="A28" s="3"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
       <c r="D28">
         <v>2018</v>
       </c>
-      <c r="E28" s="3"/>
+      <c r="E28" s="6"/>
       <c r="F28" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
+      <c r="A29" s="3"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
       <c r="D29">
         <v>2017</v>
       </c>
-      <c r="E29" s="3"/>
+      <c r="E29" s="6"/>
       <c r="F29" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
+      <c r="A30" s="3"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
       <c r="D30">
         <v>2016</v>
       </c>
-      <c r="E30" s="3"/>
+      <c r="E30" s="6"/>
       <c r="F30" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
+      <c r="A31" s="3"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
       <c r="D31">
         <v>2015</v>
       </c>
-      <c r="E31" s="3"/>
+      <c r="E31" s="6"/>
       <c r="F31" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
+      <c r="A32" s="3"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
       <c r="D32">
         <v>2014</v>
       </c>
-      <c r="E32" s="3"/>
+      <c r="E32" s="6"/>
       <c r="F32" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
+      <c r="A33" s="3"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
       <c r="D33">
         <v>2013</v>
       </c>
-      <c r="E33" s="3"/>
+      <c r="E33" s="6"/>
       <c r="F33" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
+      <c r="A34" s="3"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
       <c r="D34">
         <v>2012</v>
       </c>
-      <c r="E34" s="3"/>
+      <c r="E34" s="6"/>
       <c r="F34" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
+      <c r="A35" s="3"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
       <c r="D35">
         <v>2011</v>
       </c>
-      <c r="E35" s="3"/>
+      <c r="E35" s="6"/>
       <c r="F35" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
+      <c r="A36" s="3"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
       <c r="D36">
         <v>2010</v>
       </c>
-      <c r="E36" s="3"/>
+      <c r="E36" s="6"/>
       <c r="F36" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
+      <c r="A37" s="3"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
       <c r="D37">
         <v>2009</v>
       </c>
-      <c r="E37" s="3"/>
+      <c r="E37" s="6"/>
       <c r="F37" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
+      <c r="A38" s="3"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
       <c r="D38">
         <v>2008</v>
       </c>
-      <c r="E38" s="3"/>
+      <c r="E38" s="6"/>
       <c r="F38" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
+      <c r="A39" s="3"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
       <c r="D39">
         <v>2007</v>
       </c>
-      <c r="E39" s="3"/>
+      <c r="E39" s="6"/>
       <c r="F39" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="4"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
+      <c r="A40" s="3"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
       <c r="D40">
         <v>2006</v>
       </c>
-      <c r="E40" s="3"/>
+      <c r="E40" s="6"/>
       <c r="F40" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="4"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
+      <c r="A41" s="3"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
       <c r="D41">
         <v>2005</v>
       </c>
-      <c r="E41" s="3"/>
+      <c r="E41" s="6"/>
       <c r="F41" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="4"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
+      <c r="A42" s="3"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
       <c r="D42">
         <v>2004</v>
       </c>
-      <c r="E42" s="3"/>
+      <c r="E42" s="6"/>
       <c r="F42" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="4"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
+      <c r="A43" s="3"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
       <c r="D43">
         <v>2003</v>
       </c>
-      <c r="E43" s="3"/>
+      <c r="E43" s="6"/>
       <c r="F43" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="4"/>
-      <c r="B44" s="2" t="s">
+      <c r="A44" s="3"/>
+      <c r="B44" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C44" s="2"/>
+      <c r="C44" s="7"/>
       <c r="D44">
         <v>2020</v>
       </c>
@@ -1477,237 +1486,237 @@
       <c r="F44" t="s">
         <v>50</v>
       </c>
-      <c r="H44" s="3" t="s">
+      <c r="H44" s="6" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="4"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
+      <c r="A45" s="3"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
       <c r="D45">
         <v>2019</v>
       </c>
-      <c r="E45" s="3"/>
+      <c r="E45" s="6"/>
       <c r="F45" t="s">
         <v>35</v>
       </c>
-      <c r="H45" s="3"/>
+      <c r="H45" s="6"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="4"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
+      <c r="A46" s="3"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
       <c r="D46">
         <v>2018</v>
       </c>
-      <c r="E46" s="3"/>
+      <c r="E46" s="6"/>
       <c r="F46" t="s">
         <v>36</v>
       </c>
-      <c r="H46" s="3"/>
+      <c r="H46" s="6"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="4"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
+      <c r="A47" s="3"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
       <c r="D47">
         <v>2017</v>
       </c>
-      <c r="E47" s="3"/>
+      <c r="E47" s="6"/>
       <c r="F47" t="s">
         <v>37</v>
       </c>
-      <c r="H47" s="3"/>
+      <c r="H47" s="6"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="4"/>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
+      <c r="A48" s="3"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="7"/>
       <c r="D48">
         <v>2016</v>
       </c>
-      <c r="E48" s="3"/>
+      <c r="E48" s="6"/>
       <c r="F48" t="s">
         <v>38</v>
       </c>
-      <c r="H48" s="3"/>
+      <c r="H48" s="6"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="4"/>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
+      <c r="A49" s="3"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
       <c r="D49">
         <v>2015</v>
       </c>
-      <c r="E49" s="3"/>
+      <c r="E49" s="6"/>
       <c r="F49" t="s">
         <v>39</v>
       </c>
-      <c r="H49" s="3"/>
+      <c r="H49" s="6"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="4"/>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
+      <c r="A50" s="3"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
       <c r="D50">
         <v>2014</v>
       </c>
-      <c r="E50" s="3"/>
+      <c r="E50" s="6"/>
       <c r="F50" t="s">
         <v>40</v>
       </c>
-      <c r="H50" s="3"/>
+      <c r="H50" s="6"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="4"/>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
+      <c r="A51" s="3"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="7"/>
       <c r="D51">
         <v>2013</v>
       </c>
-      <c r="E51" s="3"/>
+      <c r="E51" s="6"/>
       <c r="F51" t="s">
         <v>41</v>
       </c>
-      <c r="H51" s="3"/>
+      <c r="H51" s="6"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="4"/>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
+      <c r="A52" s="3"/>
+      <c r="B52" s="7"/>
+      <c r="C52" s="7"/>
       <c r="D52">
         <v>2012</v>
       </c>
-      <c r="E52" s="3"/>
+      <c r="E52" s="6"/>
       <c r="F52" t="s">
         <v>42</v>
       </c>
-      <c r="H52" s="3"/>
+      <c r="H52" s="6"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="4"/>
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
+      <c r="A53" s="3"/>
+      <c r="B53" s="7"/>
+      <c r="C53" s="7"/>
       <c r="D53">
         <v>2011</v>
       </c>
-      <c r="E53" s="3"/>
+      <c r="E53" s="6"/>
       <c r="F53" t="s">
         <v>43</v>
       </c>
-      <c r="H53" s="3"/>
+      <c r="H53" s="6"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="4"/>
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
+      <c r="A54" s="3"/>
+      <c r="B54" s="7"/>
+      <c r="C54" s="7"/>
       <c r="D54">
         <v>2010</v>
       </c>
-      <c r="E54" s="3"/>
+      <c r="E54" s="6"/>
       <c r="F54" t="s">
         <v>44</v>
       </c>
-      <c r="H54" s="3"/>
+      <c r="H54" s="6"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="4"/>
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
+      <c r="A55" s="3"/>
+      <c r="B55" s="7"/>
+      <c r="C55" s="7"/>
       <c r="D55">
         <v>2009</v>
       </c>
-      <c r="E55" s="3"/>
+      <c r="E55" s="6"/>
       <c r="F55" t="s">
         <v>45</v>
       </c>
-      <c r="H55" s="3"/>
+      <c r="H55" s="6"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="4"/>
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
+      <c r="A56" s="3"/>
+      <c r="B56" s="7"/>
+      <c r="C56" s="7"/>
       <c r="D56">
         <v>2008</v>
       </c>
-      <c r="E56" s="3"/>
+      <c r="E56" s="6"/>
       <c r="F56" t="s">
         <v>46</v>
       </c>
-      <c r="H56" s="3"/>
+      <c r="H56" s="6"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="4"/>
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
+      <c r="A57" s="3"/>
+      <c r="B57" s="7"/>
+      <c r="C57" s="7"/>
       <c r="D57">
         <v>2007</v>
       </c>
-      <c r="E57" s="3"/>
+      <c r="E57" s="6"/>
       <c r="F57" t="s">
         <v>47</v>
       </c>
-      <c r="H57" s="3"/>
+      <c r="H57" s="6"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="4"/>
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
+      <c r="A58" s="3"/>
+      <c r="B58" s="7"/>
+      <c r="C58" s="7"/>
       <c r="D58">
         <v>2006</v>
       </c>
-      <c r="E58" s="3"/>
+      <c r="E58" s="6"/>
       <c r="F58" t="s">
         <v>48</v>
       </c>
-      <c r="H58" s="3"/>
+      <c r="H58" s="6"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="4"/>
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
+      <c r="A59" s="3"/>
+      <c r="B59" s="7"/>
+      <c r="C59" s="7"/>
       <c r="D59">
         <v>2005</v>
       </c>
-      <c r="E59" s="3"/>
+      <c r="E59" s="6"/>
       <c r="F59" t="s">
         <v>49</v>
       </c>
-      <c r="H59" s="3"/>
+      <c r="H59" s="6"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="4"/>
-      <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
+      <c r="A60" s="3"/>
+      <c r="B60" s="7"/>
+      <c r="C60" s="7"/>
       <c r="D60">
         <v>2004</v>
       </c>
-      <c r="E60" s="3"/>
+      <c r="E60" s="6"/>
       <c r="F60" t="s">
         <v>34</v>
       </c>
-      <c r="H60" s="3"/>
+      <c r="H60" s="6"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="4"/>
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
+      <c r="A61" s="3"/>
+      <c r="B61" s="7"/>
+      <c r="C61" s="7"/>
       <c r="D61">
         <v>2003</v>
       </c>
-      <c r="E61" s="3"/>
+      <c r="E61" s="6"/>
       <c r="F61" t="s">
         <v>33</v>
       </c>
-      <c r="H61" s="3"/>
+      <c r="H61" s="6"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="4"/>
-      <c r="B62" s="2" t="s">
+      <c r="A62" s="3"/>
+      <c r="B62" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C62" s="2"/>
+      <c r="C62" s="7"/>
       <c r="D62">
         <v>2020</v>
       </c>
@@ -1717,876 +1726,896 @@
       <c r="F62" t="s">
         <v>51</v>
       </c>
-      <c r="H62" s="3" t="s">
+      <c r="H62" s="6" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="4"/>
-      <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
+      <c r="A63" s="3"/>
+      <c r="B63" s="7"/>
+      <c r="C63" s="7"/>
       <c r="D63">
         <v>2019</v>
       </c>
-      <c r="E63" s="3"/>
+      <c r="E63" s="6"/>
       <c r="F63" t="s">
         <v>52</v>
       </c>
-      <c r="H63" s="3"/>
+      <c r="H63" s="6"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="4"/>
-      <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
+      <c r="A64" s="3"/>
+      <c r="B64" s="7"/>
+      <c r="C64" s="7"/>
       <c r="D64">
         <v>2018</v>
       </c>
-      <c r="E64" s="3"/>
+      <c r="E64" s="6"/>
       <c r="F64" t="s">
         <v>53</v>
       </c>
-      <c r="H64" s="3"/>
+      <c r="H64" s="6"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="4"/>
-      <c r="B65" s="2"/>
-      <c r="C65" s="2"/>
+      <c r="A65" s="3"/>
+      <c r="B65" s="7"/>
+      <c r="C65" s="7"/>
       <c r="D65">
         <v>2017</v>
       </c>
-      <c r="E65" s="3"/>
+      <c r="E65" s="6"/>
       <c r="F65" t="s">
         <v>54</v>
       </c>
-      <c r="H65" s="3"/>
+      <c r="H65" s="6"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="4"/>
-      <c r="B66" s="2"/>
-      <c r="C66" s="2"/>
+      <c r="A66" s="3"/>
+      <c r="B66" s="7"/>
+      <c r="C66" s="7"/>
       <c r="D66">
         <v>2016</v>
       </c>
-      <c r="E66" s="3"/>
+      <c r="E66" s="6"/>
       <c r="F66" t="s">
         <v>55</v>
       </c>
-      <c r="H66" s="3"/>
+      <c r="H66" s="6"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="4"/>
-      <c r="B67" s="2"/>
-      <c r="C67" s="2"/>
+      <c r="A67" s="3"/>
+      <c r="B67" s="7"/>
+      <c r="C67" s="7"/>
       <c r="D67">
         <v>2015</v>
       </c>
-      <c r="E67" s="3"/>
+      <c r="E67" s="6"/>
       <c r="F67" t="s">
         <v>56</v>
       </c>
-      <c r="H67" s="3"/>
+      <c r="H67" s="6"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="4"/>
-      <c r="B68" s="2"/>
-      <c r="C68" s="2"/>
+      <c r="A68" s="3"/>
+      <c r="B68" s="7"/>
+      <c r="C68" s="7"/>
       <c r="D68">
         <v>2014</v>
       </c>
-      <c r="E68" s="3"/>
+      <c r="E68" s="6"/>
       <c r="F68" t="s">
         <v>57</v>
       </c>
-      <c r="H68" s="3"/>
+      <c r="H68" s="6"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="4"/>
-      <c r="B69" s="2"/>
-      <c r="C69" s="2"/>
+      <c r="A69" s="3"/>
+      <c r="B69" s="7"/>
+      <c r="C69" s="7"/>
       <c r="D69">
         <v>2013</v>
       </c>
-      <c r="E69" s="3"/>
+      <c r="E69" s="6"/>
       <c r="F69" t="s">
         <v>58</v>
       </c>
-      <c r="H69" s="3"/>
+      <c r="H69" s="6"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="4"/>
-      <c r="B70" s="2"/>
-      <c r="C70" s="2"/>
+      <c r="A70" s="3"/>
+      <c r="B70" s="7"/>
+      <c r="C70" s="7"/>
       <c r="D70">
         <v>2012</v>
       </c>
-      <c r="E70" s="3"/>
+      <c r="E70" s="6"/>
       <c r="F70" t="s">
         <v>59</v>
       </c>
-      <c r="H70" s="3"/>
+      <c r="H70" s="6"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="4"/>
-      <c r="B71" s="2"/>
-      <c r="C71" s="2"/>
+      <c r="A71" s="3"/>
+      <c r="B71" s="7"/>
+      <c r="C71" s="7"/>
       <c r="D71">
         <v>2011</v>
       </c>
-      <c r="E71" s="3"/>
+      <c r="E71" s="6"/>
       <c r="F71" t="s">
         <v>60</v>
       </c>
-      <c r="H71" s="3"/>
+      <c r="H71" s="6"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="4"/>
-      <c r="B72" s="2"/>
-      <c r="C72" s="2"/>
+      <c r="A72" s="3"/>
+      <c r="B72" s="7"/>
+      <c r="C72" s="7"/>
       <c r="D72">
         <v>2010</v>
       </c>
-      <c r="E72" s="3"/>
+      <c r="E72" s="6"/>
       <c r="F72" t="s">
         <v>61</v>
       </c>
-      <c r="H72" s="3"/>
+      <c r="H72" s="6"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="4"/>
-      <c r="B73" s="2"/>
-      <c r="C73" s="2"/>
+      <c r="A73" s="3"/>
+      <c r="B73" s="7"/>
+      <c r="C73" s="7"/>
       <c r="D73">
         <v>2009</v>
       </c>
-      <c r="E73" s="3"/>
+      <c r="E73" s="6"/>
       <c r="F73" t="s">
         <v>62</v>
       </c>
-      <c r="H73" s="3"/>
+      <c r="H73" s="6"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="4"/>
-      <c r="B74" s="2"/>
-      <c r="C74" s="2"/>
+      <c r="A74" s="3"/>
+      <c r="B74" s="7"/>
+      <c r="C74" s="7"/>
       <c r="D74">
         <v>2008</v>
       </c>
-      <c r="E74" s="3"/>
+      <c r="E74" s="6"/>
       <c r="F74" t="s">
         <v>63</v>
       </c>
-      <c r="H74" s="3"/>
+      <c r="H74" s="6"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="4"/>
-      <c r="B75" s="2"/>
-      <c r="C75" s="2"/>
+      <c r="A75" s="3"/>
+      <c r="B75" s="7"/>
+      <c r="C75" s="7"/>
       <c r="D75">
         <v>2007</v>
       </c>
-      <c r="E75" s="3"/>
+      <c r="E75" s="6"/>
       <c r="F75" t="s">
         <v>64</v>
       </c>
-      <c r="H75" s="3"/>
+      <c r="H75" s="6"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" s="4"/>
-      <c r="B76" s="2"/>
-      <c r="C76" s="2"/>
+      <c r="A76" s="3"/>
+      <c r="B76" s="7"/>
+      <c r="C76" s="7"/>
       <c r="D76">
         <v>2006</v>
       </c>
-      <c r="E76" s="3"/>
+      <c r="E76" s="6"/>
       <c r="F76" t="s">
         <v>65</v>
       </c>
-      <c r="H76" s="3"/>
+      <c r="H76" s="6"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="4"/>
-      <c r="B77" s="2"/>
-      <c r="C77" s="2"/>
+      <c r="A77" s="3"/>
+      <c r="B77" s="7"/>
+      <c r="C77" s="7"/>
       <c r="D77">
         <v>2005</v>
       </c>
-      <c r="E77" s="3"/>
+      <c r="E77" s="6"/>
       <c r="F77" t="s">
         <v>66</v>
       </c>
-      <c r="H77" s="3"/>
+      <c r="H77" s="6"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" s="4"/>
-      <c r="B78" s="2"/>
-      <c r="C78" s="2"/>
+      <c r="A78" s="3"/>
+      <c r="B78" s="7"/>
+      <c r="C78" s="7"/>
       <c r="D78">
         <v>2004</v>
       </c>
-      <c r="E78" s="3"/>
+      <c r="E78" s="6"/>
       <c r="F78" t="s">
         <v>67</v>
       </c>
-      <c r="H78" s="3"/>
+      <c r="H78" s="6"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A79" s="4"/>
-      <c r="B79" s="2"/>
-      <c r="C79" s="2"/>
+      <c r="A79" s="3"/>
+      <c r="B79" s="7"/>
+      <c r="C79" s="7"/>
       <c r="D79">
         <v>2003</v>
       </c>
-      <c r="E79" s="3"/>
+      <c r="E79" s="6"/>
       <c r="F79" t="s">
         <v>68</v>
       </c>
-      <c r="H79" s="3"/>
+      <c r="H79" s="6"/>
     </row>
     <row r="80" spans="1:8" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="4" t="s">
+      <c r="A80" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B80" s="6" t="s">
+      <c r="B80" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C80" s="7"/>
-      <c r="D80" s="6"/>
-      <c r="E80" s="8" t="s">
+      <c r="C80" s="9"/>
+      <c r="D80" s="2"/>
+      <c r="E80" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="F80" s="6" t="s">
+      <c r="F80" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="4"/>
-      <c r="B81" s="6" t="s">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" s="3"/>
+      <c r="B81" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C81" s="7"/>
-      <c r="D81" s="6"/>
-      <c r="E81" s="8"/>
-      <c r="F81" s="6" t="s">
+      <c r="C81" s="9"/>
+      <c r="D81" s="2"/>
+      <c r="E81" s="4"/>
+      <c r="F81" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="4"/>
-      <c r="B82" s="6" t="s">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" s="3"/>
+      <c r="B82" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C82" s="7"/>
-      <c r="D82" s="6"/>
-      <c r="E82" s="8"/>
-      <c r="F82" s="6" t="s">
+      <c r="C82" s="9"/>
+      <c r="D82" s="2"/>
+      <c r="E82" s="4"/>
+      <c r="F82" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="4"/>
-      <c r="B83" s="6" t="s">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" s="3"/>
+      <c r="B83" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C83" s="7"/>
-      <c r="D83" s="6"/>
-      <c r="E83" s="8"/>
-      <c r="F83" s="6" t="s">
+      <c r="C83" s="9"/>
+      <c r="D83" s="2"/>
+      <c r="E83" s="4"/>
+      <c r="F83" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="4"/>
-      <c r="B84" s="6" t="s">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" s="3"/>
+      <c r="B84" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C84" s="7"/>
-      <c r="D84" s="6"/>
-      <c r="E84" s="8"/>
-      <c r="F84" s="6" t="s">
+      <c r="C84" s="9"/>
+      <c r="D84" s="2"/>
+      <c r="E84" s="4"/>
+      <c r="F84" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="4"/>
-      <c r="B85" s="6" t="s">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" s="3"/>
+      <c r="B85" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C85" s="7"/>
-      <c r="D85" s="6"/>
-      <c r="E85" s="8"/>
-      <c r="F85" s="6" t="s">
+      <c r="C85" s="9"/>
+      <c r="D85" s="2"/>
+      <c r="E85" s="4"/>
+      <c r="F85" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="4"/>
-      <c r="B86" s="6" t="s">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="3"/>
+      <c r="B86" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C86" s="7"/>
-      <c r="D86" s="6"/>
-      <c r="E86" s="8"/>
-      <c r="F86" s="6" t="s">
+      <c r="C86" s="9"/>
+      <c r="D86" s="2"/>
+      <c r="E86" s="4"/>
+      <c r="F86" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="4"/>
-      <c r="B87" s="6" t="s">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="3"/>
+      <c r="B87" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C87" s="7"/>
-      <c r="D87" s="6"/>
-      <c r="E87" s="8"/>
-      <c r="F87" s="6" t="s">
+      <c r="C87" s="9"/>
+      <c r="D87" s="2"/>
+      <c r="E87" s="4"/>
+      <c r="F87" s="2" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="4"/>
-      <c r="B88" s="6" t="s">
+      <c r="H87" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" s="3"/>
+      <c r="B88" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C88" s="7"/>
-      <c r="D88" s="6"/>
-      <c r="E88" s="8"/>
-      <c r="F88" s="6" t="s">
+      <c r="C88" s="9"/>
+      <c r="D88" s="2"/>
+      <c r="E88" s="4"/>
+      <c r="F88" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="4"/>
-      <c r="B89" s="6" t="s">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="3"/>
+      <c r="B89" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C89" s="9"/>
+      <c r="D89" s="2"/>
+      <c r="E89" s="4"/>
+      <c r="F89" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="3"/>
+      <c r="B90" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C89" s="7"/>
-      <c r="D89" s="6"/>
-      <c r="E89" s="8"/>
-      <c r="F89" s="6" t="s">
+      <c r="C90" s="9"/>
+      <c r="D90" s="2"/>
+      <c r="E90" s="4"/>
+      <c r="F90" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="4"/>
-      <c r="B90" s="6" t="s">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" s="3"/>
+      <c r="B91" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C90" s="7"/>
-      <c r="D90" s="6"/>
-      <c r="E90" s="8"/>
-      <c r="F90" s="6" t="s">
+      <c r="C91" s="9"/>
+      <c r="D91" s="2"/>
+      <c r="E91" s="4"/>
+      <c r="F91" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="4"/>
-      <c r="B91" s="6" t="s">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" s="3"/>
+      <c r="B92" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C91" s="7"/>
-      <c r="D91" s="6"/>
-      <c r="E91" s="8"/>
-      <c r="F91" s="6" t="s">
+      <c r="C92" s="9"/>
+      <c r="D92" s="2"/>
+      <c r="E92" s="4"/>
+      <c r="F92" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="4"/>
-      <c r="B92" s="6" t="s">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="3"/>
+      <c r="B93" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C92" s="7"/>
-      <c r="D92" s="6"/>
-      <c r="E92" s="8"/>
-      <c r="F92" s="6" t="s">
+      <c r="C93" s="9"/>
+      <c r="D93" s="2"/>
+      <c r="E93" s="4"/>
+      <c r="F93" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="4"/>
-      <c r="B93" s="6" t="s">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="3"/>
+      <c r="B94" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C93" s="7"/>
-      <c r="D93" s="6"/>
-      <c r="E93" s="8"/>
-      <c r="F93" s="6" t="s">
+      <c r="C94" s="9"/>
+      <c r="D94" s="2"/>
+      <c r="E94" s="4"/>
+      <c r="F94" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="4"/>
-      <c r="B94" s="6" t="s">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="3"/>
+      <c r="B95" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C94" s="7"/>
-      <c r="D94" s="6"/>
-      <c r="E94" s="8"/>
-      <c r="F94" s="6" t="s">
+      <c r="C95" s="9"/>
+      <c r="D95" s="2"/>
+      <c r="E95" s="4"/>
+      <c r="F95" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="4"/>
-      <c r="B95" s="6" t="s">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="3"/>
+      <c r="B96" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C95" s="7"/>
-      <c r="D95" s="6"/>
-      <c r="E95" s="8"/>
-      <c r="F95" s="6" t="s">
+      <c r="C96" s="9"/>
+      <c r="D96" s="2"/>
+      <c r="E96" s="4"/>
+      <c r="F96" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="4"/>
-      <c r="B96" s="6" t="s">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97" s="3"/>
+      <c r="B97" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C96" s="7"/>
-      <c r="D96" s="6"/>
-      <c r="E96" s="8"/>
-      <c r="F96" s="6" t="s">
+      <c r="C97" s="9"/>
+      <c r="D97" s="2"/>
+      <c r="E97" s="4"/>
+      <c r="F97" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A97" s="4"/>
-      <c r="B97" s="6" t="s">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A98" s="3"/>
+      <c r="B98" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C97" s="7"/>
-      <c r="D97" s="6"/>
-      <c r="E97" s="8"/>
-      <c r="F97" s="6" t="s">
+      <c r="C98" s="9"/>
+      <c r="D98" s="2"/>
+      <c r="E98" s="4"/>
+      <c r="F98" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A98" s="4"/>
-      <c r="B98" s="6" t="s">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A99" s="3"/>
+      <c r="B99" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C98" s="7"/>
-      <c r="D98" s="6"/>
-      <c r="E98" s="8"/>
-      <c r="F98" s="6" t="s">
+      <c r="C99" s="9"/>
+      <c r="D99" s="2"/>
+      <c r="E99" s="4"/>
+      <c r="F99" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A99" s="4"/>
-      <c r="B99" s="6" t="s">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A100" s="3"/>
+      <c r="B100" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C99" s="7"/>
-      <c r="D99" s="6"/>
-      <c r="E99" s="8"/>
-      <c r="F99" s="6" t="s">
+      <c r="C100" s="9"/>
+      <c r="D100" s="2"/>
+      <c r="E100" s="4"/>
+      <c r="F100" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A100" s="4"/>
-      <c r="B100" s="6" t="s">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A101" s="3"/>
+      <c r="B101" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C100" s="7"/>
-      <c r="D100" s="6"/>
-      <c r="E100" s="8"/>
-      <c r="F100" s="6" t="s">
+      <c r="C101" s="9"/>
+      <c r="D101" s="2"/>
+      <c r="E101" s="4"/>
+      <c r="F101" s="2" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A101" s="4"/>
-      <c r="B101" s="6" t="s">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A102" s="3"/>
+      <c r="B102" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C101" s="7"/>
-      <c r="D101" s="6"/>
-      <c r="E101" s="8"/>
-      <c r="F101" s="6"/>
-      <c r="H101" s="3" t="s">
+      <c r="C102" s="9"/>
+      <c r="D102" s="2"/>
+      <c r="E102" s="4"/>
+      <c r="F102" s="2"/>
+      <c r="H102" s="6" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A102" s="4"/>
-      <c r="B102" s="6" t="s">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A103" s="3"/>
+      <c r="B103" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C102" s="7"/>
-      <c r="D102" s="6"/>
-      <c r="E102" s="8"/>
-      <c r="F102" s="6"/>
-      <c r="H102" s="3"/>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A103" s="4"/>
-      <c r="B103" s="6" t="s">
+      <c r="C103" s="9"/>
+      <c r="D103" s="2"/>
+      <c r="E103" s="4"/>
+      <c r="F103" s="2"/>
+      <c r="H103" s="6"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A104" s="3"/>
+      <c r="B104" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C103" s="9" t="s">
+      <c r="C104" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="D103" s="6"/>
-      <c r="E103" s="8"/>
-      <c r="F103" s="6"/>
-      <c r="H103" s="3"/>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A104" s="4"/>
-      <c r="B104" s="6" t="s">
+      <c r="D104" s="2"/>
+      <c r="E104" s="4"/>
+      <c r="F104" s="2"/>
+      <c r="H104" s="6"/>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A105" s="3"/>
+      <c r="B105" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C104" s="9"/>
-      <c r="D104" s="6"/>
-      <c r="E104" s="8"/>
-      <c r="F104" s="6"/>
-      <c r="H104" s="3"/>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A105" s="4"/>
-      <c r="B105" s="6" t="s">
+      <c r="C105" s="8"/>
+      <c r="D105" s="2"/>
+      <c r="E105" s="4"/>
+      <c r="F105" s="2"/>
+      <c r="H105" s="6"/>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A106" s="3"/>
+      <c r="B106" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C105" s="7"/>
-      <c r="D105" s="6"/>
-      <c r="E105" s="8"/>
-      <c r="F105" s="6"/>
-      <c r="H105" s="3"/>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A106" s="4"/>
-      <c r="B106" s="6" t="s">
+      <c r="C106" s="9"/>
+      <c r="D106" s="2"/>
+      <c r="E106" s="4"/>
+      <c r="F106" s="2"/>
+      <c r="H106" s="6"/>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A107" s="3"/>
+      <c r="B107" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C106" s="7"/>
-      <c r="D106" s="6"/>
-      <c r="E106" s="8"/>
-      <c r="F106" s="6"/>
-      <c r="H106" s="3"/>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A107" s="4"/>
-      <c r="B107" s="6" t="s">
+      <c r="C107" s="9"/>
+      <c r="D107" s="2"/>
+      <c r="E107" s="4"/>
+      <c r="F107" s="2"/>
+      <c r="H107" s="6"/>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A108" s="3"/>
+      <c r="B108" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C107" s="7"/>
-      <c r="D107" s="6"/>
-      <c r="E107" s="8"/>
-      <c r="F107" s="6"/>
-      <c r="H107" s="3"/>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A108" s="4"/>
-      <c r="B108" s="6" t="s">
+      <c r="C108" s="9"/>
+      <c r="D108" s="2"/>
+      <c r="E108" s="4"/>
+      <c r="F108" s="2"/>
+      <c r="H108" s="6"/>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A109" s="3"/>
+      <c r="B109" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C108" s="7"/>
-      <c r="D108" s="6"/>
-      <c r="E108" s="8"/>
-      <c r="F108" s="6"/>
-      <c r="H108" s="3"/>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A109" s="4"/>
-      <c r="B109" s="6" t="s">
+      <c r="C109" s="9"/>
+      <c r="D109" s="2"/>
+      <c r="E109" s="4"/>
+      <c r="F109" s="2"/>
+      <c r="H109" s="6"/>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A110" s="3"/>
+      <c r="B110" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C109" s="7"/>
-      <c r="D109" s="6"/>
-      <c r="E109" s="8"/>
-      <c r="F109" s="6"/>
-      <c r="H109" s="3"/>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A110" s="4"/>
-      <c r="B110" s="6" t="s">
+      <c r="C110" s="9"/>
+      <c r="D110" s="2"/>
+      <c r="E110" s="4"/>
+      <c r="F110" s="2"/>
+      <c r="H110" s="6"/>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A111" s="3"/>
+      <c r="B111" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C110" s="7"/>
-      <c r="D110" s="6"/>
-      <c r="E110" s="8"/>
-      <c r="F110" s="6"/>
-      <c r="H110" s="3"/>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A111" s="4"/>
-      <c r="B111" s="6" t="s">
+      <c r="C111" s="9"/>
+      <c r="D111" s="2"/>
+      <c r="E111" s="4"/>
+      <c r="F111" s="2"/>
+      <c r="H111" s="6"/>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A112" s="3"/>
+      <c r="B112" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C111" s="7"/>
-      <c r="D111" s="6"/>
-      <c r="E111" s="8"/>
-      <c r="F111" s="6"/>
-      <c r="H111" s="3"/>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A112" s="4"/>
-      <c r="B112" s="6" t="s">
+      <c r="C112" s="9"/>
+      <c r="D112" s="2"/>
+      <c r="E112" s="4"/>
+      <c r="F112" s="2"/>
+      <c r="H112" s="6"/>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A113" s="3"/>
+      <c r="B113" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C112" s="7"/>
-      <c r="D112" s="6"/>
-      <c r="E112" s="8"/>
-      <c r="F112" s="6"/>
-      <c r="H112" s="3"/>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A113" s="4"/>
-      <c r="B113" s="6" t="s">
+      <c r="C113" s="9"/>
+      <c r="D113" s="2"/>
+      <c r="E113" s="4"/>
+      <c r="F113" s="2"/>
+      <c r="H113" s="6"/>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A114" s="3"/>
+      <c r="B114" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C113" s="7"/>
-      <c r="D113" s="6"/>
-      <c r="E113" s="8"/>
-      <c r="F113" s="6"/>
-      <c r="H113" s="3"/>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A114" s="4"/>
-      <c r="B114" s="6" t="s">
+      <c r="C114" s="9"/>
+      <c r="D114" s="2"/>
+      <c r="E114" s="4"/>
+      <c r="F114" s="2"/>
+      <c r="H114" s="6"/>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A115" s="3"/>
+      <c r="B115" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C114" s="7"/>
-      <c r="D114" s="6"/>
-      <c r="E114" s="8"/>
-      <c r="F114" s="6"/>
-      <c r="H114" s="3"/>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A115" s="4"/>
-      <c r="B115" s="6" t="s">
+      <c r="C115" s="9"/>
+      <c r="D115" s="2"/>
+      <c r="E115" s="4"/>
+      <c r="F115" s="2"/>
+      <c r="H115" s="6"/>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A116" s="3"/>
+      <c r="B116" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C115" s="7"/>
-      <c r="D115" s="6"/>
-      <c r="E115" s="8"/>
-      <c r="F115" s="6"/>
-      <c r="H115" s="3"/>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A116" s="4"/>
-      <c r="B116" s="6" t="s">
+      <c r="C116" s="9"/>
+      <c r="D116" s="2"/>
+      <c r="E116" s="4"/>
+      <c r="F116" s="2"/>
+      <c r="H116" s="6"/>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A117" s="3"/>
+      <c r="B117" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C116" s="7"/>
-      <c r="D116" s="6"/>
-      <c r="E116" s="8"/>
-      <c r="F116" s="6"/>
-      <c r="H116" s="3"/>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A117" s="4"/>
-      <c r="B117" s="6" t="s">
+      <c r="C117" s="9"/>
+      <c r="D117" s="2"/>
+      <c r="E117" s="4"/>
+      <c r="F117" s="2"/>
+      <c r="H117" s="6"/>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A118" s="3"/>
+      <c r="B118" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C117" s="7"/>
-      <c r="D117" s="6"/>
-      <c r="E117" s="8"/>
-      <c r="F117" s="6"/>
-      <c r="H117" s="3"/>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A118" s="4"/>
-      <c r="B118" s="6" t="s">
+      <c r="C118" s="9"/>
+      <c r="D118" s="2"/>
+      <c r="E118" s="4"/>
+      <c r="F118" s="2"/>
+      <c r="H118" s="6"/>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A119" s="3"/>
+      <c r="B119" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C118" s="7"/>
-      <c r="D118" s="6"/>
-      <c r="E118" s="8"/>
-      <c r="F118" s="6"/>
-      <c r="H118" s="3"/>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A119" s="4"/>
-      <c r="B119" s="6" t="s">
+      <c r="C119" s="9"/>
+      <c r="D119" s="2"/>
+      <c r="E119" s="4"/>
+      <c r="F119" s="2"/>
+      <c r="H119" s="6"/>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A120" s="3"/>
+      <c r="B120" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C119" s="7"/>
-      <c r="D119" s="6"/>
-      <c r="E119" s="8"/>
-      <c r="F119" s="6"/>
-      <c r="H119" s="3"/>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
+      <c r="C120" s="9"/>
+      <c r="D120" s="2"/>
+      <c r="E120" s="4"/>
+      <c r="F120" s="2"/>
+      <c r="H120" s="6"/>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
         <v>119</v>
       </c>
-      <c r="B120" s="6" t="s">
+      <c r="B121" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C120" s="6"/>
-      <c r="D120" s="6">
+      <c r="C121" s="2"/>
+      <c r="D121" s="2">
         <v>2011</v>
       </c>
-      <c r="E120" s="8"/>
-      <c r="F120" s="6" t="s">
+      <c r="E121" s="4"/>
+      <c r="F121" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="121" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="3" t="s">
+    <row r="122" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="B121" t="s">
+      <c r="B122" t="s">
         <v>144</v>
       </c>
-      <c r="C121" s="1"/>
-      <c r="D121" s="2">
+      <c r="C122" s="1"/>
+      <c r="D122" s="7">
         <v>2017</v>
       </c>
-      <c r="E121" s="3" t="s">
+      <c r="E122" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="F121" t="s">
+      <c r="F122" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A122" s="3"/>
-      <c r="B122" t="s">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A123" s="6"/>
+      <c r="B123" t="s">
         <v>145</v>
       </c>
-      <c r="C122" s="1"/>
-      <c r="D122" s="2"/>
-      <c r="E122" s="3"/>
-      <c r="F122" t="s">
+      <c r="C123" s="1"/>
+      <c r="D123" s="7"/>
+      <c r="E123" s="6"/>
+      <c r="F123" t="s">
         <v>148</v>
       </c>
-      <c r="H122" t="s">
+      <c r="H123" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A123" s="3"/>
-      <c r="B123" t="s">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A124" s="6"/>
+      <c r="B124" t="s">
         <v>146</v>
       </c>
-      <c r="C123" s="1"/>
-      <c r="D123" s="2"/>
-      <c r="E123" s="3"/>
-      <c r="F123" t="s">
+      <c r="C124" s="1"/>
+      <c r="D124" s="7"/>
+      <c r="E124" s="6"/>
+      <c r="F124" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A124" s="3"/>
-      <c r="B124" t="s">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A125" s="6"/>
+      <c r="B125" t="s">
         <v>152</v>
       </c>
-      <c r="D124" s="2">
+      <c r="D125" s="7">
         <v>2015</v>
       </c>
-      <c r="E124" s="3" t="s">
+      <c r="E125" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="F124" t="s">
+      <c r="F125" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A125" s="3"/>
-      <c r="B125" t="s">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A126" s="6"/>
+      <c r="B126" t="s">
         <v>153</v>
       </c>
-      <c r="D125" s="2"/>
-      <c r="E125" s="3"/>
-      <c r="F125" t="s">
+      <c r="D126" s="7"/>
+      <c r="E126" s="6"/>
+      <c r="F126" t="s">
         <v>148</v>
       </c>
-      <c r="H125" t="s">
+      <c r="H126" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A126" s="3"/>
-      <c r="B126" t="s">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A127" s="6"/>
+      <c r="B127" t="s">
         <v>157</v>
       </c>
-      <c r="D126" s="2"/>
-      <c r="E126" t="s">
+      <c r="D127" s="7"/>
+      <c r="E127" t="s">
         <v>155</v>
       </c>
-      <c r="F126" t="s">
+      <c r="F127" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A127" s="3"/>
-      <c r="B127" t="s">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A128" s="6"/>
+      <c r="B128" t="s">
         <v>159</v>
       </c>
-      <c r="D127" s="2">
+      <c r="D128" s="7">
         <v>2013</v>
       </c>
-      <c r="E127" s="2" t="s">
+      <c r="E128" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="F127" t="s">
+      <c r="F128" t="s">
         <v>149</v>
       </c>
-      <c r="H127" t="s">
+      <c r="H128" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A128" s="3"/>
-      <c r="B128" t="s">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A129" s="6"/>
+      <c r="B129" t="s">
         <v>160</v>
       </c>
-      <c r="D128" s="2"/>
-      <c r="E128" s="2"/>
-      <c r="F128" t="s">
+      <c r="D129" s="7"/>
+      <c r="E129" s="7"/>
+      <c r="F129" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A129" s="3"/>
-      <c r="B129" t="s">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A130" s="6"/>
+      <c r="B130" t="s">
         <v>158</v>
       </c>
-      <c r="D129" s="2">
+      <c r="D130" s="7">
         <v>2008</v>
       </c>
-      <c r="E129" s="2" t="s">
+      <c r="E130" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="F129" t="s">
+      <c r="F130" t="s">
         <v>164</v>
       </c>
-      <c r="H129" t="s">
+      <c r="H130" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A130" s="3"/>
-      <c r="B130" t="s">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A131" s="6"/>
+      <c r="B131" t="s">
         <v>165</v>
       </c>
-      <c r="D130" s="2"/>
-      <c r="E130" s="2"/>
-      <c r="F130" t="s">
+      <c r="D131" s="7"/>
+      <c r="E131" s="7"/>
+      <c r="F131" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A131" s="3"/>
-      <c r="D131" s="1"/>
-      <c r="E131" s="1"/>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A132" s="6"/>
+      <c r="D132" s="1"/>
+      <c r="E132" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="A80:A119"/>
-    <mergeCell ref="E80:E120"/>
-    <mergeCell ref="E44:E61"/>
-    <mergeCell ref="B44:B61"/>
-    <mergeCell ref="C44:C61"/>
-    <mergeCell ref="B62:B79"/>
-    <mergeCell ref="C62:C79"/>
-    <mergeCell ref="E62:E79"/>
+    <mergeCell ref="E130:E131"/>
+    <mergeCell ref="A122:A132"/>
+    <mergeCell ref="E122:E124"/>
+    <mergeCell ref="D122:D124"/>
+    <mergeCell ref="D125:D127"/>
+    <mergeCell ref="E125:E126"/>
+    <mergeCell ref="D128:D129"/>
+    <mergeCell ref="D130:D131"/>
+    <mergeCell ref="H102:H120"/>
+    <mergeCell ref="C80:C86"/>
+    <mergeCell ref="C87:C101"/>
+    <mergeCell ref="C102:C103"/>
+    <mergeCell ref="E128:E129"/>
     <mergeCell ref="H44:H61"/>
     <mergeCell ref="H62:H79"/>
     <mergeCell ref="A2:A4"/>
@@ -2600,29 +2629,24 @@
     <mergeCell ref="C5:C25"/>
     <mergeCell ref="C2:C4"/>
     <mergeCell ref="E26:E43"/>
-    <mergeCell ref="C103:C104"/>
-    <mergeCell ref="C105:C112"/>
-    <mergeCell ref="C113:C119"/>
-    <mergeCell ref="H101:H119"/>
-    <mergeCell ref="C80:C86"/>
-    <mergeCell ref="C87:C100"/>
-    <mergeCell ref="C101:C102"/>
-    <mergeCell ref="E127:E128"/>
-    <mergeCell ref="E129:E130"/>
-    <mergeCell ref="A121:A131"/>
-    <mergeCell ref="E121:E123"/>
-    <mergeCell ref="D121:D123"/>
-    <mergeCell ref="D124:D126"/>
-    <mergeCell ref="E124:E125"/>
-    <mergeCell ref="D127:D128"/>
-    <mergeCell ref="D129:D130"/>
+    <mergeCell ref="A80:A120"/>
+    <mergeCell ref="E80:E121"/>
+    <mergeCell ref="E44:E61"/>
+    <mergeCell ref="B44:B61"/>
+    <mergeCell ref="C44:C61"/>
+    <mergeCell ref="B62:B79"/>
+    <mergeCell ref="C62:C79"/>
+    <mergeCell ref="E62:E79"/>
+    <mergeCell ref="C104:C105"/>
+    <mergeCell ref="C106:C113"/>
+    <mergeCell ref="C114:C120"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="E26" r:id="rId1" xr:uid="{0231060C-331E-4465-A525-FE5D78DEE5A9}"/>
     <hyperlink ref="E44" r:id="rId2" xr:uid="{E2F22A19-392A-4865-B7BB-4C304D93753E}"/>
     <hyperlink ref="E62" r:id="rId3" xr:uid="{79496A2A-90DD-4614-9A89-9DB620F55616}"/>
-    <hyperlink ref="B120" r:id="rId4" display="https://www.cbs.gov.il/he/publications/LochutTlushim/2021/%D7%A8%D7%97%D7%95%D7%91%D7%95%D7%AA %D7%A2%D7%99%D7%A7%D7%A8%D7%99%D7%99%D7%9D %D7%95%D7%A9%D7%9B%D7%95%D7%A0%D7%95%D7%AA %D7%9C%D7%90%D7%A1 2011.xlsx" xr:uid="{2FC3E2A6-E097-478E-AF83-C103BD3826E9}"/>
+    <hyperlink ref="B121" r:id="rId4" display="https://www.cbs.gov.il/he/publications/LochutTlushim/2021/%D7%A8%D7%97%D7%95%D7%91%D7%95%D7%AA %D7%A2%D7%99%D7%A7%D7%A8%D7%99%D7%99%D7%9D %D7%95%D7%A9%D7%9B%D7%95%D7%A0%D7%95%D7%AA %D7%9C%D7%90%D7%A1 2011.xlsx" xr:uid="{2FC3E2A6-E097-478E-AF83-C103BD3826E9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>